<commit_message>
Interactive map and table.
</commit_message>
<xml_diff>
--- a/data/parks.xlsx
+++ b/data/parks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/petrusn_uef_fi/Documents/3_fun_code/vaellus/finnish-national-parks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FECD8684-FF19-4D8B-9A59-8354DF4B79B5}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5618EDC0-0745-4DD8-A4EA-3018F19D5DBF}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="199">
   <si>
     <t>Etelä-Konneveden kansallispuisto</t>
   </si>
   <si>
-    <t>31 000</t>
-  </si>
-  <si>
     <t>Helvetinjärven kansallispuisto</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>Ruovesi</t>
   </si>
   <si>
-    <t>44 000</t>
-  </si>
-  <si>
     <t>Hiidenportin kansallispuisto</t>
   </si>
   <si>
@@ -54,72 +48,45 @@
     <t>Sotkamo</t>
   </si>
   <si>
-    <t>9 800</t>
-  </si>
-  <si>
     <t>Hossan kansallispuisto</t>
   </si>
   <si>
-    <t>77 900</t>
-  </si>
-  <si>
     <t>Isojärven kansallispuisto</t>
   </si>
   <si>
     <t>Kuhmoinen</t>
   </si>
   <si>
-    <t>24 300</t>
-  </si>
-  <si>
     <t>Itäisen Suomenlahden kansallispuisto</t>
   </si>
   <si>
     <t>Kymenlaakso</t>
   </si>
   <si>
-    <t>15 800</t>
-  </si>
-  <si>
     <t>Kauhanevan–Pohjankankaan kansallispuisto</t>
   </si>
   <si>
-    <t>26 300</t>
-  </si>
-  <si>
     <t>Kolin kansallispuisto</t>
   </si>
   <si>
     <t>Pohjois-Karjala</t>
   </si>
   <si>
-    <t>249 100</t>
-  </si>
-  <si>
     <t>Koloveden kansallispuisto</t>
   </si>
   <si>
-    <t>14 200</t>
-  </si>
-  <si>
     <t>Kurjenrahkan kansallispuisto</t>
   </si>
   <si>
     <t>Varsinais-Suomi</t>
   </si>
   <si>
-    <t>67 300</t>
-  </si>
-  <si>
     <t>Lauhanvuoren kansallispuisto</t>
   </si>
   <si>
     <t>Etelä-Pohjanmaa</t>
   </si>
   <si>
-    <t>21 300</t>
-  </si>
-  <si>
     <t>Leivonmäen kansallispuisto</t>
   </si>
   <si>
@@ -129,195 +96,114 @@
     <t>Joutsa</t>
   </si>
   <si>
-    <t>28 700</t>
-  </si>
-  <si>
     <t>Lemmenjoen kansallispuisto</t>
   </si>
   <si>
     <t>Lappi</t>
   </si>
   <si>
-    <t>23 900</t>
-  </si>
-  <si>
     <t>Liesjärven kansallispuisto</t>
   </si>
   <si>
-    <t>50 400</t>
-  </si>
-  <si>
     <t>Linnansaaren kansallispuisto</t>
   </si>
   <si>
-    <t>39 200</t>
-  </si>
-  <si>
     <t>Nuuksion kansallispuisto</t>
   </si>
   <si>
     <t>Uusimaa</t>
   </si>
   <si>
-    <t>274 400</t>
-  </si>
-  <si>
     <t>Oulangan kansallispuisto</t>
   </si>
   <si>
-    <t>175 800</t>
-  </si>
-  <si>
     <t>Pallas-Yllästunturin kansallispuisto</t>
   </si>
   <si>
-    <t>584 000</t>
-  </si>
-  <si>
     <t>Patvinsuon kansallispuisto</t>
   </si>
   <si>
-    <t>16 500</t>
-  </si>
-  <si>
     <t>Perämeren kansallispuisto</t>
   </si>
   <si>
-    <t>6 400</t>
-  </si>
-  <si>
     <t>Petkeljärven kansallispuisto</t>
   </si>
   <si>
     <t>Ilomantsi</t>
   </si>
   <si>
-    <t>16 100</t>
-  </si>
-  <si>
     <t>Puurijärven ja Isosuon kansallispuisto</t>
   </si>
   <si>
-    <t>20 200</t>
-  </si>
-  <si>
     <t>Pyhä-Häkin kansallispuisto</t>
   </si>
   <si>
     <t>Saarijärvi</t>
   </si>
   <si>
-    <t>18 400</t>
-  </si>
-  <si>
     <t>Pyhä-Luoston kansallispuisto</t>
   </si>
   <si>
-    <t>217 400</t>
-  </si>
-  <si>
     <t>Päijänteen kansallispuisto</t>
   </si>
   <si>
     <t>Päijät-Häme</t>
   </si>
   <si>
-    <t>67 000</t>
-  </si>
-  <si>
     <t>Repoveden kansallispuisto</t>
   </si>
   <si>
-    <t>132 400</t>
-  </si>
-  <si>
     <t>Riisitunturin kansallispuisto</t>
   </si>
   <si>
     <t>Posio</t>
   </si>
   <si>
-    <t>61 200</t>
-  </si>
-  <si>
     <t>Rokuan kansallispuisto</t>
   </si>
   <si>
     <t>Pohjois-Pohjanmaa</t>
   </si>
   <si>
-    <t>47 700</t>
-  </si>
-  <si>
     <t>Saaristomeren kansallispuisto</t>
   </si>
   <si>
-    <t>78 800</t>
-  </si>
-  <si>
     <t>Salamajärven kansallispuisto</t>
   </si>
   <si>
-    <t>25 300</t>
-  </si>
-  <si>
     <t>Sallan kansallispuisto</t>
   </si>
   <si>
     <t>Salla</t>
   </si>
   <si>
-    <t>62 200</t>
-  </si>
-  <si>
     <t>Seitsemisen kansallispuisto</t>
   </si>
   <si>
-    <t>43 600</t>
-  </si>
-  <si>
     <t>Selkämeren kansallispuisto</t>
   </si>
   <si>
-    <t>79 400</t>
-  </si>
-  <si>
     <t>Sipoonkorven kansallispuisto</t>
   </si>
   <si>
-    <t>172 500</t>
-  </si>
-  <si>
     <t>Syötteen kansallispuisto</t>
   </si>
   <si>
-    <t>106 100</t>
-  </si>
-  <si>
     <t>Tammisaaren saariston kansallispuisto</t>
   </si>
   <si>
     <t>Raasepori</t>
   </si>
   <si>
-    <t>53 200</t>
-  </si>
-  <si>
     <t>Teijon kansallispuisto</t>
   </si>
   <si>
     <t>Salo</t>
   </si>
   <si>
-    <t>93 000</t>
-  </si>
-  <si>
     <t>Tiilikkajärven kansallispuisto</t>
   </si>
   <si>
-    <t>24 700</t>
-  </si>
-  <si>
     <t>Torronsuon kansallispuisto</t>
   </si>
   <si>
@@ -327,19 +213,10 @@
     <t>Tammela</t>
   </si>
   <si>
-    <t>58 000</t>
-  </si>
-  <si>
     <t>Urho Kekkosen kansallispuisto</t>
   </si>
   <si>
-    <t>417 600</t>
-  </si>
-  <si>
     <t>Valkmusan kansallispuisto</t>
-  </si>
-  <si>
-    <t>20 000</t>
   </si>
   <si>
     <t>Pohjois-Savo ja Keski-Suomi</t>
@@ -796,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -822,11 +699,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,10 +991,10 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,40 +1005,40 @@
     <col min="4" max="4" width="26.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="11" customWidth="1"/>
     <col min="8" max="16384" width="18" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>166</v>
+        <v>107</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1166,13 +1046,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="E2" s="5">
         <v>15.44</v>
@@ -1180,28 +1060,28 @@
       <c r="F2" s="8">
         <v>2014</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>1</v>
+      <c r="G2" s="9">
+        <v>31000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="E3" s="5">
         <v>49.5</v>
@@ -1209,28 +1089,28 @@
       <c r="F3" s="8">
         <v>1982</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>5</v>
+      <c r="G3" s="9">
+        <v>44000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="5">
         <v>45</v>
@@ -1238,28 +1118,28 @@
       <c r="F4" s="8">
         <v>1982</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>9</v>
+      <c r="G4" s="9">
+        <v>9800</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>202</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E5" s="5">
         <v>110</v>
@@ -1267,28 +1147,28 @@
       <c r="F5" s="8">
         <v>2017</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>11</v>
+      <c r="G5" s="9">
+        <v>77900</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5">
         <v>22</v>
@@ -1296,28 +1176,28 @@
       <c r="F6" s="8">
         <v>1982</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>14</v>
+      <c r="G6" s="9">
+        <v>24300</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>204</v>
+        <v>163</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="E7" s="5">
         <v>7</v>
@@ -1325,28 +1205,28 @@
       <c r="F7" s="8">
         <v>1982</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>17</v>
+      <c r="G7" s="9">
+        <v>15800</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="E8" s="5">
         <v>57</v>
@@ -1354,28 +1234,28 @@
       <c r="F8" s="8">
         <v>1982</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>19</v>
+      <c r="G8" s="9">
+        <v>26300</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>206</v>
+        <v>165</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E9" s="5">
         <v>30</v>
@@ -1383,28 +1263,28 @@
       <c r="F9" s="8">
         <v>1991</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>22</v>
+      <c r="G9" s="9">
+        <v>249100</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="E10" s="5">
         <v>23</v>
@@ -1412,28 +1292,28 @@
       <c r="F10" s="8">
         <v>1990</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>24</v>
+      <c r="G10" s="9">
+        <v>14200</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5">
         <v>29</v>
@@ -1441,28 +1321,28 @@
       <c r="F11" s="8">
         <v>1998</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>27</v>
+      <c r="G11" s="9">
+        <v>67300</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="E12" s="5">
         <v>54</v>
@@ -1470,28 +1350,28 @@
       <c r="F12" s="8">
         <v>1982</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>30</v>
+      <c r="G12" s="9">
+        <v>21300</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5">
         <v>30</v>
@@ -1499,28 +1379,28 @@
       <c r="F13" s="8">
         <v>2003</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>34</v>
+      <c r="G13" s="9">
+        <v>28700</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="E14" s="5">
         <v>2860</v>
@@ -1528,28 +1408,28 @@
       <c r="F14" s="8">
         <v>1956</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>37</v>
+      <c r="G14" s="9">
+        <v>23900</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5">
         <v>22</v>
@@ -1557,28 +1437,28 @@
       <c r="F15" s="8">
         <v>1956</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>39</v>
+      <c r="G15" s="9">
+        <v>50400</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5">
         <v>96</v>
@@ -1586,28 +1466,28 @@
       <c r="F16" s="8">
         <v>1956</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>41</v>
+      <c r="G16" s="9">
+        <v>39200</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="E17" s="5">
         <v>53</v>
@@ -1615,28 +1495,28 @@
       <c r="F17" s="8">
         <v>1994</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>44</v>
+      <c r="G17" s="9">
+        <v>274400</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E18" s="5">
         <v>290</v>
@@ -1644,28 +1524,28 @@
       <c r="F18" s="8">
         <v>1956</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>46</v>
+      <c r="G18" s="9">
+        <v>175800</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="E19" s="5">
         <v>1020</v>
@@ -1673,28 +1553,28 @@
       <c r="F19" s="8">
         <v>1938</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>48</v>
+      <c r="G19" s="9">
+        <v>584000</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="E20" s="5">
         <v>105</v>
@@ -1702,28 +1582,28 @@
       <c r="F20" s="8">
         <v>1982</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>50</v>
+      <c r="G20" s="9">
+        <v>16500</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="E21" s="5">
         <v>157</v>
@@ -1731,28 +1611,28 @@
       <c r="F21" s="8">
         <v>1991</v>
       </c>
-      <c r="G21" s="10" t="s">
-        <v>52</v>
+      <c r="G21" s="9">
+        <v>6400</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E22" s="5">
         <v>6</v>
@@ -1760,28 +1640,28 @@
       <c r="F22" s="8">
         <v>1956</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>55</v>
+      <c r="G22" s="9">
+        <v>16100</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="E23" s="5">
         <v>27</v>
@@ -1789,28 +1669,28 @@
       <c r="F23" s="8">
         <v>1993</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>57</v>
+      <c r="G23" s="9">
+        <v>20200</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="E24" s="5">
         <v>13</v>
@@ -1818,28 +1698,28 @@
       <c r="F24" s="8">
         <v>1956</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>60</v>
+      <c r="G24" s="9">
+        <v>18400</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>222</v>
+        <v>181</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="E25" s="5">
         <v>142</v>
@@ -1847,28 +1727,28 @@
       <c r="F25" s="8">
         <v>1938</v>
       </c>
-      <c r="G25" s="10" t="s">
-        <v>62</v>
+      <c r="G25" s="9">
+        <v>217400</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>223</v>
+        <v>182</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="E26" s="5">
         <v>14</v>
@@ -1876,28 +1756,28 @@
       <c r="F26" s="8">
         <v>1993</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>65</v>
+      <c r="G26" s="9">
+        <v>67000</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>224</v>
+        <v>183</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="E27" s="5">
         <v>15</v>
@@ -1905,28 +1785,28 @@
       <c r="F27" s="8">
         <v>2003</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>67</v>
+      <c r="G27" s="9">
+        <v>132400</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="E28" s="5">
         <v>76</v>
@@ -1934,28 +1814,28 @@
       <c r="F28" s="8">
         <v>1982</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>70</v>
+      <c r="G28" s="9">
+        <v>61200</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="E29" s="5">
         <v>15</v>
@@ -1963,28 +1843,28 @@
       <c r="F29" s="8">
         <v>1956</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>73</v>
+      <c r="G29" s="9">
+        <v>47700</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="E30" s="5">
         <v>500</v>
@@ -1992,28 +1872,28 @@
       <c r="F30" s="8">
         <v>1983</v>
       </c>
-      <c r="G30" s="10" t="s">
-        <v>75</v>
+      <c r="G30" s="9">
+        <v>78800</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>228</v>
+        <v>187</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="E31" s="5">
         <v>62</v>
@@ -2021,28 +1901,28 @@
       <c r="F31" s="8">
         <v>1982</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>77</v>
+      <c r="G31" s="9">
+        <v>25300</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E32" s="5">
         <v>99.83</v>
@@ -2050,25 +1930,28 @@
       <c r="F32" s="8">
         <v>2022</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>80</v>
+      <c r="G32" s="9">
+        <v>62200</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>191</v>
+        <v>150</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="E33" s="5">
         <v>45.5</v>
@@ -2076,28 +1959,28 @@
       <c r="F33" s="8">
         <v>1982</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>82</v>
+      <c r="G33" s="9">
+        <v>43600</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>230</v>
+        <v>189</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="E34" s="5">
         <v>913</v>
@@ -2105,28 +1988,28 @@
       <c r="F34" s="8">
         <v>2011</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>84</v>
+      <c r="G34" s="9">
+        <v>79400</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="E35" s="5">
         <v>24</v>
@@ -2134,28 +2017,28 @@
       <c r="F35" s="8">
         <v>2011</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>86</v>
+      <c r="G35" s="9">
+        <v>172500</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="E36" s="5">
         <v>299</v>
@@ -2163,28 +2046,28 @@
       <c r="F36" s="8">
         <v>2000</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>88</v>
+      <c r="G36" s="9">
+        <v>106100</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="E37" s="5">
         <v>52</v>
@@ -2192,28 +2075,28 @@
       <c r="F37" s="8">
         <v>1989</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>91</v>
+      <c r="G37" s="9">
+        <v>53200</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E38" s="5">
         <v>33.85</v>
@@ -2221,28 +2104,28 @@
       <c r="F38" s="8">
         <v>2015</v>
       </c>
-      <c r="G38" s="10" t="s">
-        <v>94</v>
+      <c r="G38" s="9">
+        <v>93000</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="E39" s="5">
         <v>71</v>
@@ -2250,28 +2133,28 @@
       <c r="F39" s="8">
         <v>1982</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>96</v>
+      <c r="G39" s="9">
+        <v>24700</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E40" s="5">
         <v>30</v>
@@ -2279,28 +2162,28 @@
       <c r="F40" s="8">
         <v>1990</v>
       </c>
-      <c r="G40" s="10" t="s">
-        <v>100</v>
+      <c r="G40" s="9">
+        <v>58000</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="E41" s="5">
         <v>2550</v>
@@ -2308,28 +2191,28 @@
       <c r="F41" s="8">
         <v>1983</v>
       </c>
-      <c r="G41" s="10" t="s">
-        <v>102</v>
+      <c r="G41" s="9">
+        <v>417600</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="E42" s="5">
         <v>19.5</v>
@@ -2337,14 +2220,14 @@
       <c r="F42" s="8">
         <v>1996</v>
       </c>
-      <c r="G42" s="10" t="s">
-        <v>104</v>
+      <c r="G42" s="9">
+        <v>20000</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added visit dates (month/year)
</commit_message>
<xml_diff>
--- a/data/parks.xlsx
+++ b/data/parks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/petrusn_uef_fi/Documents/3_fun_code/vaellus/finnish-national-parks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5618EDC0-0745-4DD8-A4EA-3018F19D5DBF}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B4EFF6E-250B-4CB9-9F79-20F558D3E7D6}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="214">
   <si>
     <t>Etelä-Konneveden kansallispuisto</t>
   </si>
@@ -375,9 +375,6 @@
     <t>Visit</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>62.5500, 26.6333</t>
   </si>
   <si>
@@ -622,6 +619,54 @@
   </si>
   <si>
     <t>Park_short</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>6/2019</t>
+  </si>
+  <si>
+    <t>6/2020</t>
+  </si>
+  <si>
+    <t>7/2019</t>
+  </si>
+  <si>
+    <t>7/2020</t>
+  </si>
+  <si>
+    <t>10/2019</t>
+  </si>
+  <si>
+    <t>2/2020</t>
+  </si>
+  <si>
+    <t>8/2020</t>
+  </si>
+  <si>
+    <t>6/2021</t>
+  </si>
+  <si>
+    <t>2016, 2017, 9/2018, 3/2019, 9/2021, 10/2021</t>
+  </si>
+  <si>
+    <t>7/2022</t>
+  </si>
+  <si>
+    <t>9/2022</t>
+  </si>
+  <si>
+    <t>12/2020, 9/2022</t>
+  </si>
+  <si>
+    <t>8/2023</t>
+  </si>
+  <si>
+    <t>8/2019, 9/2020, 7/2023, 7/2024</t>
+  </si>
+  <si>
+    <t>8/2024</t>
   </si>
 </sst>
 </file>
@@ -673,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -707,6 +752,12 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,10 +1042,10 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1057,9 @@
     <col min="5" max="5" width="10.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="18" style="2"/>
+    <col min="8" max="9" width="18" style="2"/>
+    <col min="10" max="10" width="59.5703125" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="18" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1014,7 +1067,7 @@
         <v>108</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>110</v>
@@ -1029,7 +1082,7 @@
         <v>107</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>114</v>
@@ -1037,8 +1090,8 @@
       <c r="I1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>116</v>
+      <c r="J1" s="12" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1046,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -1064,10 +1117,13 @@
         <v>31000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1075,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -1093,10 +1149,13 @@
         <v>44000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1104,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1122,10 +1181,13 @@
         <v>9800</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1133,7 +1195,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>66</v>
@@ -1151,10 +1213,13 @@
         <v>77900</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1162,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -1180,10 +1245,10 @@
         <v>24300</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1191,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -1209,10 +1274,10 @@
         <v>15800</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1220,7 +1285,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>69</v>
@@ -1238,10 +1303,13 @@
         <v>26300</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,7 +1317,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1267,10 +1335,13 @@
         <v>249100</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,7 +1349,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>72</v>
@@ -1296,10 +1367,13 @@
         <v>14200</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1307,7 +1381,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
@@ -1325,10 +1399,10 @@
         <v>67300</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1336,7 +1410,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
@@ -1354,10 +1428,13 @@
         <v>21300</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1365,7 +1442,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
@@ -1383,10 +1460,13 @@
         <v>28700</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1394,7 +1474,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>24</v>
@@ -1412,10 +1492,10 @@
         <v>23900</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1423,7 +1503,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>77</v>
@@ -1441,10 +1521,13 @@
         <v>50400</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1452,7 +1535,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>79</v>
@@ -1470,18 +1553,18 @@
         <v>39200</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>28</v>
@@ -1499,18 +1582,21 @@
         <v>274400</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>82</v>
@@ -1528,18 +1614,21 @@
         <v>175800</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
@@ -1557,18 +1646,21 @@
         <v>584000</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1586,18 +1678,21 @@
         <v>16500</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>24</v>
@@ -1615,18 +1710,18 @@
         <v>6400</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
@@ -1644,18 +1739,18 @@
         <v>16100</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>87</v>
@@ -1673,18 +1768,18 @@
         <v>20200</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
@@ -1702,18 +1797,21 @@
         <v>18400</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>24</v>
@@ -1731,18 +1829,21 @@
         <v>217400</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>40</v>
@@ -1760,18 +1861,18 @@
         <v>67000</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>91</v>
@@ -1789,18 +1890,18 @@
         <v>132400</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>24</v>
@@ -1818,18 +1919,21 @@
         <v>61200</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>45</v>
@@ -1847,18 +1951,18 @@
         <v>47700</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
@@ -1876,18 +1980,18 @@
         <v>78800</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>95</v>
@@ -1905,13 +2009,16 @@
         <v>25300</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1934,18 +2041,18 @@
         <v>62200</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2</v>
@@ -1963,18 +2070,18 @@
         <v>43600</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>98</v>
@@ -1992,18 +2099,18 @@
         <v>79400</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>28</v>
@@ -2021,18 +2128,21 @@
         <v>172500</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>82</v>
@@ -2050,18 +2160,21 @@
         <v>106100</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>28</v>
@@ -2079,18 +2192,18 @@
         <v>53200</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>17</v>
@@ -2108,18 +2221,18 @@
         <v>93000</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>102</v>
@@ -2137,18 +2250,21 @@
         <v>24700</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>60</v>
@@ -2169,15 +2285,18 @@
         <v>113</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>24</v>
@@ -2200,13 +2319,16 @@
       <c r="I41" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>11</v>
@@ -2227,7 +2349,10 @@
         <v>111</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added .gpx routes to the map.
</commit_message>
<xml_diff>
--- a/data/parks.xlsx
+++ b/data/parks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/petrusn_uef_fi/Documents/3_fun_code/vaellus/finnish-national-parks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="291" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B4EFF6E-250B-4CB9-9F79-20F558D3E7D6}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="11_AD4D1D646341095ACB7000854554F87E683EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBBBD452-ED21-4375-A00A-100B43F1709A}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -648,9 +648,6 @@
     <t>6/2021</t>
   </si>
   <si>
-    <t>2016, 2017, 9/2018, 3/2019, 9/2021, 10/2021</t>
-  </si>
-  <si>
     <t>7/2022</t>
   </si>
   <si>
@@ -667,6 +664,9 @@
   </si>
   <si>
     <t>8/2024</t>
+  </si>
+  <si>
+    <t>2016, 2017, 9/2018, 3/2019, 9/2021, 10/2021, 10/2024</t>
   </si>
 </sst>
 </file>
@@ -1045,24 +1045,24 @@
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="37.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="11" customWidth="1"/>
     <col min="8" max="9" width="18" style="2"/>
-    <col min="10" max="10" width="59.5703125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="59.5546875" style="13" customWidth="1"/>
     <col min="11" max="16384" width="18" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>108</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1123,10 +1123,10 @@
         <v>134</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1341,10 +1341,10 @@
         <v>134</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1466,10 +1466,10 @@
         <v>134</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -1620,10 +1620,10 @@
         <v>134</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1652,10 +1652,10 @@
         <v>134</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -1835,10 +1835,10 @@
         <v>134</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1925,10 +1925,10 @@
         <v>134</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>53</v>
       </c>
@@ -2166,10 +2166,10 @@
         <v>134</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>54</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>58</v>
       </c>
@@ -2256,10 +2256,10 @@
         <v>134</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>59</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>62</v>
       </c>
@@ -2320,10 +2320,10 @@
         <v>134</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added Repovesi and 2nd visit to Syöte (old, 2024). And modified the seasonal figure.
</commit_message>
<xml_diff>
--- a/data/parks.xlsx
+++ b/data/parks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/petrusn_uef_fi/Documents/3_fun_code/vaellus/finnish-national-parks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{378AD10D-A084-4049-B39D-923DF47C7264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1E6251-ABAB-4BF9-BC5E-A8154ACFDCB0}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{378AD10D-A084-4049-B39D-923DF47C7264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1F2D1A9-8EE7-4A45-B9C8-0CFBD45DECCB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="237">
   <si>
     <t>Etelä-Konneveden kansallispuisto</t>
   </si>
@@ -665,9 +665,6 @@
     <t>12/2020, 9/2022</t>
   </si>
   <si>
-    <t>8/2023</t>
-  </si>
-  <si>
     <t>8/2019, 9/2020, 7/2023, 7/2024</t>
   </si>
   <si>
@@ -744,6 +741,12 @@
   </si>
   <si>
     <t>12/2025</t>
+  </si>
+  <si>
+    <t>2/2026</t>
+  </si>
+  <si>
+    <t>8/2023, 8/2024</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1125,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1153,7 @@
         <v>109</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>108</v>
@@ -1185,7 +1188,7 @@
         <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -1220,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
@@ -1255,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -1290,7 +1293,7 @@
         <v>65</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>66</v>
@@ -1325,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -1357,7 +1360,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>67</v>
@@ -1380,7 +1383,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>162</v>
@@ -1389,7 +1392,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>69</v>
@@ -1424,7 +1427,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>70</v>
@@ -1445,7 +1448,7 @@
         <v>133</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1459,7 +1462,7 @@
         <v>71</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>72</v>
@@ -1494,7 +1497,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>73</v>
@@ -1526,7 +1529,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>74</v>
@@ -1561,7 +1564,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>21</v>
@@ -1596,7 +1599,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>75</v>
@@ -1628,7 +1631,7 @@
         <v>76</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>77</v>
@@ -1663,7 +1666,7 @@
         <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>79</v>
@@ -1695,7 +1698,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>80</v>
@@ -1730,7 +1733,7 @@
         <v>81</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>82</v>
@@ -1765,7 +1768,7 @@
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>83</v>
@@ -1800,7 +1803,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>84</v>
@@ -1835,7 +1838,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>85</v>
@@ -1856,7 +1859,7 @@
         <v>133</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1870,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>33</v>
@@ -1891,7 +1894,7 @@
         <v>133</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1905,7 +1908,7 @@
         <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>87</v>
@@ -1937,7 +1940,7 @@
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>36</v>
@@ -1972,7 +1975,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>88</v>
@@ -2007,7 +2010,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>89</v>
@@ -2039,7 +2042,7 @@
         <v>90</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>91</v>
@@ -2057,7 +2060,10 @@
         <v>143</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2071,7 +2077,7 @@
         <v>23</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>42</v>
@@ -2106,7 +2112,7 @@
         <v>44</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>92</v>
@@ -2127,7 +2133,7 @@
         <v>133</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2141,7 +2147,7 @@
         <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>93</v>
@@ -2173,7 +2179,7 @@
         <v>94</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>95</v>
@@ -2208,7 +2214,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>48</v>
@@ -2240,7 +2246,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>96</v>
@@ -2272,7 +2278,7 @@
         <v>97</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>98</v>
@@ -2304,7 +2310,7 @@
         <v>27</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>99</v>
@@ -2339,7 +2345,7 @@
         <v>81</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>100</v>
@@ -2360,7 +2366,7 @@
         <v>133</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2374,7 +2380,7 @@
         <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>54</v>
@@ -2406,7 +2412,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>56</v>
@@ -2438,7 +2444,7 @@
         <v>101</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>102</v>
@@ -2459,7 +2465,7 @@
         <v>133</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2473,7 +2479,7 @@
         <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>60</v>
@@ -2508,7 +2514,7 @@
         <v>23</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>103</v>
@@ -2529,7 +2535,7 @@
         <v>133</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2543,7 +2549,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>104</v>
@@ -2569,19 +2575,19 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F43" s="6">
         <v>1151</v>
@@ -2590,30 +2596,30 @@
         <v>1980</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>133</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F44" s="6">
         <v>134</v>
@@ -2622,7 +2628,7 @@
         <v>1970</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>133</v>
@@ -2633,19 +2639,19 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="F45" s="6">
         <v>77</v>
@@ -2654,13 +2660,13 @@
         <v>1909</v>
       </c>
       <c r="I45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K45" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K45" s="11" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>